<commit_message>
Bugged allmetrics, please change filename so you dont save over graphs
</commit_message>
<xml_diff>
--- a/Final_Draft_Position_Graphs.xlsx
+++ b/Final_Draft_Position_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7072BD-8939-4D96-83FE-DA5B157D1A84}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A204C5-166A-4703-949D-48D405D3052F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" tabRatio="881" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" tabRatio="881" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustered Normalized Metrics" sheetId="16" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <sheet name="Fantasy Pts vs DraftPos" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -979,7 +978,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E6BF4C4-05BA-4E85-98C3-5FABC8204D66}" type="CELLRANGE">
+                    <a:fld id="{94416AE9-822C-4EEF-9DA2-9FCE8FAC8AF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1013,7 +1012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0727C15B-E8AB-4B64-B1EB-7EEE20EA0D94}" type="CELLRANGE">
+                    <a:fld id="{3C22A7A4-E15B-4CC5-975A-60D907AD0112}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1047,7 +1046,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{141922F4-CB16-4A93-8682-9F5593390059}" type="CELLRANGE">
+                    <a:fld id="{586B9C4A-354F-4907-A3B3-6879D2842B58}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1081,7 +1080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA8498B8-ACE2-4964-BF5F-F61044B1604D}" type="CELLRANGE">
+                    <a:fld id="{5036ACDC-388D-44E2-9013-6DC6475C21CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1115,7 +1114,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96955814-275C-4C1A-8D9D-EA09051C252F}" type="CELLRANGE">
+                    <a:fld id="{4648BC33-0B7F-49E3-AB9F-7FB301A175D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1149,7 +1148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B691378-B791-4C58-9B2C-579037DDAE07}" type="CELLRANGE">
+                    <a:fld id="{286EF292-8F91-4A36-869E-5288C796D930}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4725,7 +4724,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40D1ED27-8DA0-4ABB-8BCE-A8E92550AD41}" type="CELLRANGE">
+                    <a:fld id="{D479198A-0BDB-4774-8362-AF154EDAC0F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4759,7 +4758,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EBCE311-2773-4C69-BDD8-6B77830182E6}" type="CELLRANGE">
+                    <a:fld id="{D838CACB-B153-4B4A-B157-738C13C7B671}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4793,7 +4792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80CFB1E6-2D14-4050-A25C-D0B875C6B7E0}" type="CELLRANGE">
+                    <a:fld id="{F1394FBB-33F2-4F85-87BD-9424612A3D00}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4827,7 +4826,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EF5E864-A961-4E0C-B38E-9BFA56B5282B}" type="CELLRANGE">
+                    <a:fld id="{0A010D4A-AF88-4378-A1B3-23AEF83020E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4861,7 +4860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C712AEB9-F660-4F68-9659-43B2A7BBD7F3}" type="CELLRANGE">
+                    <a:fld id="{7F4B68A1-EDEE-4F38-8108-16B3FD1E6CDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4895,7 +4894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03AE71A8-8CB4-4448-80F4-A3C45CE7477F}" type="CELLRANGE">
+                    <a:fld id="{464F31F3-3300-4517-8730-51D9F5285FA4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5437,7 +5436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C3C1C1C-D216-4A3A-B310-3F1FE3FB6E61}" type="CELLRANGE">
+                    <a:fld id="{8FC80F79-F131-4C04-A43D-207687AC9200}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5471,7 +5470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08F9EACB-D03F-4322-9332-C6A46A5F0072}" type="CELLRANGE">
+                    <a:fld id="{FC15BF6E-91F3-48F1-92D9-788998D2CE20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5505,7 +5504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17EDCFE3-17A3-4AAD-AA1B-2BA52DF3BCCD}" type="CELLRANGE">
+                    <a:fld id="{233E1EB0-4749-48E3-A0F4-602DD246F186}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5539,7 +5538,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7076701-99F1-4752-AF11-259107240F48}" type="CELLRANGE">
+                    <a:fld id="{2A484D97-4C00-41CF-AEC7-CDD5F38118D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5573,7 +5572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{705222FB-A5F9-4745-9D5B-9499619C8D10}" type="CELLRANGE">
+                    <a:fld id="{00DA3D91-F043-4613-B7EA-B7BE6BB825F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5607,7 +5606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{614D912F-E97D-4FDB-89F4-95E2F4630DF0}" type="CELLRANGE">
+                    <a:fld id="{C8B5099E-F1D9-4374-86F0-B1276472DEA7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5641,7 +5640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32D35615-4598-4AC2-870F-22386188AF73}" type="CELLRANGE">
+                    <a:fld id="{AC81939F-82C7-4ECC-A252-5CC006F2679A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5675,7 +5674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33588C1D-F942-4E3C-90CF-67EF7525F63F}" type="CELLRANGE">
+                    <a:fld id="{66750CCC-79AC-4C6E-AFBD-4969BC8C1914}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5709,7 +5708,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{346B3774-EC96-44FD-BCB2-A2D9F10E91DD}" type="CELLRANGE">
+                    <a:fld id="{C0EBC327-3222-402F-9ACC-5A1C56181283}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5743,7 +5742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A2946C2-5769-4834-BCC0-CCC0FF4F3C54}" type="CELLRANGE">
+                    <a:fld id="{572829F6-53E7-4DC4-83E2-EFC80EC19DFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5777,7 +5776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A26E9EDC-85F8-40A3-8C24-4E398613C48D}" type="CELLRANGE">
+                    <a:fld id="{BF91CD63-A278-44DD-8E19-3DED42A4815D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5811,7 +5810,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3C30A4E-57AE-4F89-99F0-65FF123D6BE8}" type="CELLRANGE">
+                    <a:fld id="{B1B9A4E4-DEBA-4A81-829D-10B607EDA162}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5845,7 +5844,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E4F53E6-162E-49C6-B8FC-69289E31491D}" type="CELLRANGE">
+                    <a:fld id="{C93A3E95-A296-4B05-A9AF-3038AC578803}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5879,7 +5878,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4A60A0C-C543-47AA-987A-2EFF1A5C21B8}" type="CELLRANGE">
+                    <a:fld id="{2887F905-2B5D-4A61-928D-346CCA999FEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5913,7 +5912,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3CF7E23F-777C-4F28-A49D-8A0BC844A132}" type="CELLRANGE">
+                    <a:fld id="{1CFD2306-6D21-4D83-9072-A836B94965A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5947,7 +5946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{645A9D40-EFB2-4612-BF13-A688703A3530}" type="CELLRANGE">
+                    <a:fld id="{74210ABE-415B-46A6-9EE3-711DB37AF5F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5981,7 +5980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C562B855-4439-4D0E-B239-EF16428A606A}" type="CELLRANGE">
+                    <a:fld id="{19683799-4ECD-484B-B7EF-D1BBEA17E823}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6015,7 +6014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9B785FD-3B6A-4F9E-BA8F-3D0EF64BB7DE}" type="CELLRANGE">
+                    <a:fld id="{675361C6-29A1-4396-B547-281ACB4ECF1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6049,7 +6048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB333C83-0A15-4EEC-8A43-1F6D5FDAECC7}" type="CELLRANGE">
+                    <a:fld id="{696AD6CD-B400-4742-A7CA-5ECCD1C34561}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6083,7 +6082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DBB67CF-9DE9-490C-B871-4FCA88426B7C}" type="CELLRANGE">
+                    <a:fld id="{D1B64284-3C10-4C60-BAAF-AC16C8CC370C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6117,7 +6116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A494838F-4EA9-4FC1-80C9-AABA44672431}" type="CELLRANGE">
+                    <a:fld id="{E5819031-7430-4838-A7F2-22CC8FE2B0E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6151,7 +6150,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24ED84B7-72AF-46E4-A991-1BF3CE9F41FF}" type="CELLRANGE">
+                    <a:fld id="{8D532238-0822-41C7-A404-E437BEDA31D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6185,7 +6184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D262F3A1-40D7-4A75-9B0D-B627B4D0B63C}" type="CELLRANGE">
+                    <a:fld id="{9C094F49-466B-43BC-B0D7-0F15E903966B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6219,7 +6218,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD02227A-A0EF-470F-90E5-AB51C5D8A1C9}" type="CELLRANGE">
+                    <a:fld id="{CA9B6F99-071F-4AC3-96D6-47E6FD78ED7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6253,7 +6252,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{310C2EA2-0879-4BBD-88DF-7F5C8923B141}" type="CELLRANGE">
+                    <a:fld id="{378248C6-EC9C-4D2F-8410-FEEB7D855D39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6287,7 +6286,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{094040E0-5DC9-407C-8DD4-8D60F233F139}" type="CELLRANGE">
+                    <a:fld id="{A27E2E7E-338C-4270-8BB4-12E058B15927}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6321,7 +6320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12B46AA4-DF01-412D-8133-A114CD662652}" type="CELLRANGE">
+                    <a:fld id="{47646426-DB3D-4CFD-BE75-7BA2A5D17617}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6355,7 +6354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA2C012C-BD34-490A-9E7C-CF036E8A21C5}" type="CELLRANGE">
+                    <a:fld id="{4762EB56-5E07-44D4-B046-34F7563FC461}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6389,7 +6388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{048C25D2-A49D-40B8-A51E-25F530573583}" type="CELLRANGE">
+                    <a:fld id="{7603B40B-36E6-41DC-B94B-49AB8D7EEC45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6423,7 +6422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CFE9BE0-2EB9-40F4-8557-0FC1371516BB}" type="CELLRANGE">
+                    <a:fld id="{357D27D6-B52C-4338-B7E7-1BDE8E145C4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6457,7 +6456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83915B2E-1991-4C59-8EBF-41B6181BE595}" type="CELLRANGE">
+                    <a:fld id="{12DB852E-D5FB-4A2B-B7A5-A9BE1FFAC475}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6491,7 +6490,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C600AA84-C37B-41EF-BFC9-B4EEF3428F30}" type="CELLRANGE">
+                    <a:fld id="{3ED8FB63-BDE4-4FB5-A988-E3C062654285}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6525,7 +6524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E1D3E9F-6361-4596-8CF9-8B8AC9513F97}" type="CELLRANGE">
+                    <a:fld id="{337FD06B-C6CC-4902-A88F-E4CAB1848A49}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6559,7 +6558,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9457222-FDD3-4B4D-BC38-496E6D0C2DCC}" type="CELLRANGE">
+                    <a:fld id="{0C45A75F-A61C-46D6-A5B3-A0C1AB30C8BB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6593,7 +6592,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65C3B369-DA84-40DD-A4F1-6E302968D39A}" type="CELLRANGE">
+                    <a:fld id="{4E9BF6F5-5DB2-4E10-85C5-B886DFC1B1AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6627,7 +6626,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D96A846F-EED2-4858-9976-5BFA569CAD26}" type="CELLRANGE">
+                    <a:fld id="{5494E0E3-67BF-4D0C-BFA2-C67D41639848}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6661,7 +6660,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81BCDA27-F0B6-494C-8692-246195DE65DA}" type="CELLRANGE">
+                    <a:fld id="{CCF7A066-C01C-4532-9D5A-AFC266FA43BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6695,7 +6694,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73ED218A-6F7C-4FFF-96F9-D4E5EC1FA6EB}" type="CELLRANGE">
+                    <a:fld id="{5357A749-B12D-49F4-8968-6E337AE6B92A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6729,7 +6728,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCC30F03-892B-448E-9864-4763ED72D25F}" type="CELLRANGE">
+                    <a:fld id="{5F8524E9-E4F0-4212-82AE-633E0859A8EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6763,7 +6762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{052443BD-4DF0-492F-A3CF-83E9276C31A3}" type="CELLRANGE">
+                    <a:fld id="{43B7F7B6-BDE4-4A55-A83D-7136D945C4E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6797,7 +6796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACCD7E36-9BAE-4116-8AF5-90EC7A3517E4}" type="CELLRANGE">
+                    <a:fld id="{0C28720A-4239-4DA2-A222-FB305B2ACDC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6831,7 +6830,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{671FFA07-8411-413A-A679-76DB0A5065BB}" type="CELLRANGE">
+                    <a:fld id="{B4EFC6FF-FFE1-40A7-8DBD-F5A111D5BCBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6865,7 +6864,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AE61ECA-16F6-4319-8EA6-4A7150C255E3}" type="CELLRANGE">
+                    <a:fld id="{665E44CE-18C0-47C5-A6FD-13AEB2F01DEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6899,7 +6898,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B9363EF-0471-4F8F-BC3F-9B06E7F8FF20}" type="CELLRANGE">
+                    <a:fld id="{204683DD-5189-40AB-B414-C4410B87C7C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6933,7 +6932,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8882D85C-8B82-4133-BA6D-1BF4F549A810}" type="CELLRANGE">
+                    <a:fld id="{9AFABC14-4399-458A-9E84-7EFDE545A2BB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6967,7 +6966,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E78133FB-2476-4362-B2E3-77F88E00C2C3}" type="CELLRANGE">
+                    <a:fld id="{36790B19-C0B4-4D31-A923-B8B0303326DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7001,7 +7000,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56BDA7A4-3A80-490E-B82F-BA7713F57867}" type="CELLRANGE">
+                    <a:fld id="{2B3A2CDC-FDBA-40DF-AE58-487C09D9A3D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7035,7 +7034,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{889E4109-A240-4573-AE14-A942FB532613}" type="CELLRANGE">
+                    <a:fld id="{1988E395-363E-4463-974D-629F497694AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7069,7 +7068,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6680A095-41D9-4C59-B742-09754EDAA32F}" type="CELLRANGE">
+                    <a:fld id="{3060224E-20D4-4EF2-98A1-4592B7A1F44C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7103,7 +7102,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D879546-5A92-4784-AD8C-06149C1C7F67}" type="CELLRANGE">
+                    <a:fld id="{6E9EEAA4-EE60-414A-A7C0-D43691E41762}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7137,7 +7136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBF17EBF-3091-4A75-8233-46430EC226A7}" type="CELLRANGE">
+                    <a:fld id="{7D62E27E-41F4-4950-81BA-C3AC3364BAA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7171,7 +7170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E863E8E-E7EE-4AC4-AB7B-230F56586B20}" type="CELLRANGE">
+                    <a:fld id="{844733F1-BBAE-4CCC-8B4F-D14491A8FA86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7205,7 +7204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4044534-D5A6-4F3E-94D6-2104A679AB58}" type="CELLRANGE">
+                    <a:fld id="{4C5ADCFC-B1B3-4866-BB18-59D8E1B67468}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7239,7 +7238,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9EB14D5-0722-477E-A781-7CF11D788DC5}" type="CELLRANGE">
+                    <a:fld id="{7A3AE7C6-27FB-4F41-8F69-A05D4372847E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7273,7 +7272,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16025DA2-3E5D-4C58-81EA-C9DDD804909B}" type="CELLRANGE">
+                    <a:fld id="{AEDFD575-13A2-443E-BE42-AA459213FBE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7307,7 +7306,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04C77C4B-7A5F-4175-96C0-475B46DC9CBA}" type="CELLRANGE">
+                    <a:fld id="{41D29C7D-B7ED-4DE3-9C14-B1F355F83877}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7341,7 +7340,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B834014-4A6F-4E39-8A49-F22E911C9FC1}" type="CELLRANGE">
+                    <a:fld id="{EF99F997-0F34-42E8-BB2B-722AB81302F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7375,7 +7374,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{832F9C21-0FEA-4422-BF38-651897646682}" type="CELLRANGE">
+                    <a:fld id="{DA4BA4E1-EF99-465A-A93C-FEEA4A233555}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7409,7 +7408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5FD304D-BF1D-4C0D-9EE4-786F0C5C7EDA}" type="CELLRANGE">
+                    <a:fld id="{D00EF8CD-83A2-4B9F-8854-055C6386B875}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7443,7 +7442,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E72469B4-2ED8-4360-8576-FDD36F63D49E}" type="CELLRANGE">
+                    <a:fld id="{13C6A4EA-0F4E-48B1-9FA3-C880C08AA79C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8576,7 +8575,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{163BCDF1-48D9-42C1-A907-8FD493167EF5}" type="CELLRANGE">
+                    <a:fld id="{AED4DA74-0043-43CB-951F-E25731C825DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8610,7 +8609,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A2226CB-3AA8-4990-8306-98597EFB980A}" type="CELLRANGE">
+                    <a:fld id="{8D0A1DD8-73C2-4EDA-BF57-CFEA2E45A02A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8644,7 +8643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{898F38B4-484A-4D28-9CAC-2996CF212FDF}" type="CELLRANGE">
+                    <a:fld id="{35CA49B0-B87A-4EC7-8CDA-18AD0B02355F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8678,7 +8677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{844E1122-3CC9-4039-9476-7BAF3CCF25C4}" type="CELLRANGE">
+                    <a:fld id="{AA3EAD88-F42F-4F70-B8F5-B0548EEB8335}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8712,7 +8711,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCDBF4C2-A8FB-4372-A5D8-70F519C28A35}" type="CELLRANGE">
+                    <a:fld id="{CF414876-D338-4138-802F-963F8F2E840C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8746,7 +8745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D024288-EDF4-4598-96C5-08AD3C981383}" type="CELLRANGE">
+                    <a:fld id="{2E02D5EA-058E-4623-8C8B-B313C0BBA0A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8780,7 +8779,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB766E59-A85C-4E7C-94CA-BC1236A37660}" type="CELLRANGE">
+                    <a:fld id="{3524CA98-3A0D-4676-AC9C-74BAB3E88103}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8814,7 +8813,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF03DEA3-FFAD-4B43-8BDA-7BF4743216AB}" type="CELLRANGE">
+                    <a:fld id="{898BFE0C-DAE6-4E50-86AB-50E76F1A71ED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8848,7 +8847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACA75C4F-1F38-464E-AAB2-89F4A2214887}" type="CELLRANGE">
+                    <a:fld id="{303F6B98-FA17-4586-9ED1-917851689F95}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8882,7 +8881,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7CEB06D-73D0-4F9C-B177-EF0CAE657851}" type="CELLRANGE">
+                    <a:fld id="{6AAC30A3-D56E-471E-872C-313074083B3E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8916,7 +8915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFD0541F-1667-41AB-A57C-353CC7AD09C8}" type="CELLRANGE">
+                    <a:fld id="{28587279-E79A-4262-95A8-157D175CEEE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8950,7 +8949,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5ACAF9C-2F99-4BB6-8E87-9B59E911233D}" type="CELLRANGE">
+                    <a:fld id="{E17FB05B-0F32-4674-9EE2-AB76CF34E846}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8984,7 +8983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED796B48-AE58-4712-B7EB-E291A64DA61F}" type="CELLRANGE">
+                    <a:fld id="{233F7079-EC09-40C7-8738-940DF2C95F65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9018,7 +9017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91743BB8-8B54-4998-B1F7-3EB3B6C38524}" type="CELLRANGE">
+                    <a:fld id="{CB450193-37CD-4A4D-B4E8-77319D216326}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9052,7 +9051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BD51C29-3671-4604-BCA1-F39DFBDF35B3}" type="CELLRANGE">
+                    <a:fld id="{B0F38783-FA3C-4D57-81E3-6B9AB79A27A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9086,7 +9085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{138E4251-CBAA-4C85-B66A-8E3BAD97B273}" type="CELLRANGE">
+                    <a:fld id="{A2F377AA-85AB-40E9-B674-255F736B32E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9120,7 +9119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B358111-0CA0-4876-9671-9B6A1B282F29}" type="CELLRANGE">
+                    <a:fld id="{58E0364C-1A33-4E25-AC91-2743A0AFD740}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9154,7 +9153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDB00B96-4582-4975-AEDA-3E24961F5DD1}" type="CELLRANGE">
+                    <a:fld id="{CE9E1C52-AD88-4CDB-B854-1B5D1D08B608}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9188,7 +9187,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{654385B3-7C6E-4DCF-8492-2EDC3BBC08A4}" type="CELLRANGE">
+                    <a:fld id="{10316184-E105-4DAF-8CA4-DA2C3C40F368}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9222,7 +9221,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A69571D4-1006-4D35-832B-CD6B723428C0}" type="CELLRANGE">
+                    <a:fld id="{8C67A479-8CAD-48DE-A123-6E280E40AE16}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9256,7 +9255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AF3A4B7-47F8-4006-8D2E-A32AE473C707}" type="CELLRANGE">
+                    <a:fld id="{D048334B-7D97-4D6F-9CD1-DD32AF07774B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9290,7 +9289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36B0F782-4077-4233-9122-CB8E363E6098}" type="CELLRANGE">
+                    <a:fld id="{E79DA0B1-3039-4F43-855C-1F3315FECF87}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9324,7 +9323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D270457-9C1B-4655-9864-365EF704A06C}" type="CELLRANGE">
+                    <a:fld id="{31D42F0C-3A09-4E77-92F1-0D1E9641B80A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9358,7 +9357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45936057-20BF-4910-A21F-B560A54C197D}" type="CELLRANGE">
+                    <a:fld id="{B8066F8E-C846-4564-AC0A-8576FBD31A58}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9392,7 +9391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{518AC3A0-6147-4CDE-A7CB-56A24F15A791}" type="CELLRANGE">
+                    <a:fld id="{87791645-F59F-4351-9191-9DBED00F36D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9426,7 +9425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6426255-456C-45B2-801E-67AE45B83A96}" type="CELLRANGE">
+                    <a:fld id="{AF4B71C9-71FB-44D1-A03E-1EB3CF8AB0AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9460,7 +9459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78A2B49C-D878-4094-8DED-B338CA4C7F68}" type="CELLRANGE">
+                    <a:fld id="{1DD89B80-B2EE-4B20-813A-5E80377269E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9494,7 +9493,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A6236DE-7C33-48F7-9E8F-4976A2DD7141}" type="CELLRANGE">
+                    <a:fld id="{06077433-B221-4CD7-9464-69ED810572FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9528,7 +9527,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C8FA997-D5DE-41BF-8157-A160C2AB81B4}" type="CELLRANGE">
+                    <a:fld id="{DADF137A-C0C9-4E68-9D75-EAFFDC21248B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9562,7 +9561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F32EFBC5-D6BE-4C13-B61F-6F6E8A6F8371}" type="CELLRANGE">
+                    <a:fld id="{19E734D8-065F-46DC-8470-D3586A2FE03E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9596,7 +9595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EE80A36-7CEF-45FD-99D3-2DACDBD951D2}" type="CELLRANGE">
+                    <a:fld id="{D7233302-3D8E-496C-84DC-61AFC4B1DDE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9630,7 +9629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18E17B02-FF09-406B-A11D-63D0B8041907}" type="CELLRANGE">
+                    <a:fld id="{15559151-B54B-466E-98F3-5B6483F66A0D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9664,7 +9663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E74D8FF-CC06-4963-844B-350C1EF509B4}" type="CELLRANGE">
+                    <a:fld id="{A1778B2D-CD5A-4478-B927-1D160F73F5B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9698,7 +9697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87B7F223-A5E6-47CA-81D8-23B671D3C745}" type="CELLRANGE">
+                    <a:fld id="{16232DED-4B0F-4416-9852-93B99F8CE897}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9732,7 +9731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3EC49B3-4135-4236-A8BE-BBA9F6BF8DA2}" type="CELLRANGE">
+                    <a:fld id="{18DC0E3F-19F0-4A49-BFE3-8CD79743A9D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9766,7 +9765,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B443256-FD7C-443E-A918-3B9629420F40}" type="CELLRANGE">
+                    <a:fld id="{9367DCF2-8115-4C47-BC5D-122E397C4BAA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9800,7 +9799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9A5C936-F43C-4414-84A6-76A26AC008BD}" type="CELLRANGE">
+                    <a:fld id="{E6A5B48B-7D4E-40FE-8EBE-7339840CF55E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9834,7 +9833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3325C0A4-1F6B-401C-9DBE-DC469BB62ED0}" type="CELLRANGE">
+                    <a:fld id="{D62FC753-4228-42A0-8DBB-48B1F3BAD6EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9868,7 +9867,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E51D7DD0-0621-4109-95F1-82FFE5532A98}" type="CELLRANGE">
+                    <a:fld id="{B9AA4C18-5A40-467D-9705-F8CD518DE7C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9902,7 +9901,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B9149E1-D3A1-43F6-A63D-19A90BA3AD47}" type="CELLRANGE">
+                    <a:fld id="{2CFB60A2-FC9B-473F-ACA7-A10DCADB131C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9936,7 +9935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7BE6515-6F9E-4A97-A8AD-BFCF23E5E374}" type="CELLRANGE">
+                    <a:fld id="{73B5B843-AB4B-4372-9B70-B5922D820083}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9970,7 +9969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45E45FAD-0F65-4DD1-AB1C-B1D15CED69FE}" type="CELLRANGE">
+                    <a:fld id="{7508CC4F-0AB0-4C2F-BD76-C3D1616B7F66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10004,7 +10003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B1588F8-C84E-43E6-BEA0-54B1B4130D15}" type="CELLRANGE">
+                    <a:fld id="{2BFFA34E-35D7-443D-A034-B1C76401537E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10038,7 +10037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{652CB3F5-9F90-4DBC-8B73-B7B66E6151A9}" type="CELLRANGE">
+                    <a:fld id="{8D6C5563-BD0A-4431-AC33-2663F901CF4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10072,7 +10071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{094EF158-201E-4437-8A45-2292F95CDF26}" type="CELLRANGE">
+                    <a:fld id="{4BF2BC08-694D-4994-93D4-5CD0FF7F88B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10106,7 +10105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB9B8F5B-2971-4783-AB26-F3F47E8DD7D0}" type="CELLRANGE">
+                    <a:fld id="{582C12F7-9983-484B-9108-79171F7CDDBC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10140,7 +10139,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C705669F-48BB-43EC-951A-2A2D5E51CA67}" type="CELLRANGE">
+                    <a:fld id="{C9F219ED-C72B-4134-8A77-72220897B8A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10174,7 +10173,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1DB3E7A-154F-4B0B-822B-27CB0C3FCF47}" type="CELLRANGE">
+                    <a:fld id="{E549D023-C07B-465B-B3E3-CBB78AF1448D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10208,7 +10207,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C06028C1-8F21-4AA4-92CB-377E3E2EADCF}" type="CELLRANGE">
+                    <a:fld id="{D5EAE8EC-510F-489E-A597-B1E354178F56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10242,7 +10241,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8491B1EE-EE3D-434B-8CEB-BCE728A26753}" type="CELLRANGE">
+                    <a:fld id="{4265AAC5-CCF4-4F72-923B-D7968EB839D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10276,7 +10275,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFAD66AF-7206-44AD-A528-97C3B43B2531}" type="CELLRANGE">
+                    <a:fld id="{2A9292BB-DA22-45EC-BB75-32FCA9C9AD8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10310,7 +10309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1A39C3A-10B0-4C03-A08D-50A17260F931}" type="CELLRANGE">
+                    <a:fld id="{B8EA126A-D061-4262-A52B-9587233FD089}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10344,7 +10343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90BB6FAA-D4F3-4B0B-B3EC-A5D19B48E157}" type="CELLRANGE">
+                    <a:fld id="{8B939CE1-BAA4-4B6C-8644-86A5278D0414}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10378,7 +10377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B60D09E-9679-41FF-8BC0-4880714B0628}" type="CELLRANGE">
+                    <a:fld id="{28F763A7-4E78-4ACA-A9E7-D40343DB66C7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10412,7 +10411,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D1E4DFB-06D7-406F-962B-CD8D1333E6AC}" type="CELLRANGE">
+                    <a:fld id="{168180E3-ECAD-4F54-8952-6E68FAA32EA0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10446,7 +10445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{343856E4-4D95-4717-82BF-BD34B1B806E4}" type="CELLRANGE">
+                    <a:fld id="{7D41B78E-EFBC-4040-8E16-EFE19D6573DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10480,7 +10479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E45CFCA5-1B2D-4213-9C56-62193986E184}" type="CELLRANGE">
+                    <a:fld id="{E36DB5AC-4E67-4EBD-A4A1-9D7D8366E10B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10514,7 +10513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBA0D7DF-9034-4028-8D84-82DCFE2E446B}" type="CELLRANGE">
+                    <a:fld id="{A139CB5A-A63C-4C2F-A9BD-3A8DBBF995BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10548,7 +10547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4479C067-0727-4CF5-A06C-535EDE0310C4}" type="CELLRANGE">
+                    <a:fld id="{298191E3-06FC-4903-AC71-E55B77B178CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10582,7 +10581,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2B02931-981A-41A6-8975-2E4B3B951420}" type="CELLRANGE">
+                    <a:fld id="{3D70EE90-9BD7-461B-A778-1F614401DF5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11712,7 +11711,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D3F3356-A058-493D-BB00-6848352D473C}" type="CELLRANGE">
+                    <a:fld id="{70FA5CE7-D2D8-490E-A2CF-7D6E3361D4D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11746,7 +11745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F3139A3-9DA1-4EFB-A938-310BB8B8E6AA}" type="CELLRANGE">
+                    <a:fld id="{CE4B5821-6DF1-42A8-AD6B-25403EF98B5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11780,7 +11779,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E70C6A6-B471-42A3-9446-46AAF5F21511}" type="CELLRANGE">
+                    <a:fld id="{709025D2-F4EC-408C-AC70-6C413AFECB4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11814,7 +11813,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A10E066-4A5B-4823-B1D2-7998B278ABF7}" type="CELLRANGE">
+                    <a:fld id="{8446301A-14A5-4BE8-9E5B-18DD7571CC21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11848,7 +11847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1106F4A6-4F8D-4423-B2E1-E80A78F46342}" type="CELLRANGE">
+                    <a:fld id="{210FF9E8-9AED-4947-978D-87E06ECBF595}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11882,7 +11881,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53192C46-D39B-465A-A61A-00065D00C952}" type="CELLRANGE">
+                    <a:fld id="{90EEF6DE-2595-4ED4-A5E2-F45AA82FE7FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11916,7 +11915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{306D1DD8-DF8E-4980-BBC6-CF4ACCB00DB1}" type="CELLRANGE">
+                    <a:fld id="{76C29AC2-184F-406A-9676-E6A48E68C88A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11950,7 +11949,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F32B0BAD-80ED-4C0F-8558-0395C2AF8A34}" type="CELLRANGE">
+                    <a:fld id="{1CF36CB5-BB49-4ABE-94FF-C53A07D2E7F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11984,7 +11983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC919F93-5EA0-4097-B1FA-01657EF770C3}" type="CELLRANGE">
+                    <a:fld id="{8907A4CF-832C-44A4-9E10-7A7B7BB77B32}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12018,7 +12017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE52DC16-11B2-4D1E-9F22-20B0041E2592}" type="CELLRANGE">
+                    <a:fld id="{2616CBCA-1AD8-48DB-B9C1-D1616E1E4DD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12052,7 +12051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3103A90B-69F3-469A-8068-3747D3E7BFF1}" type="CELLRANGE">
+                    <a:fld id="{DC9F266B-51BA-425E-8E23-AD93C0120D7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12086,7 +12085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46CDB437-3CB4-4586-B083-BF49B01AD2B6}" type="CELLRANGE">
+                    <a:fld id="{F16AA954-AE70-4A5E-A82B-8F21365F3B2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12120,7 +12119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A8E9F57-2056-4442-A14E-E4C1129188E7}" type="CELLRANGE">
+                    <a:fld id="{1BA516A6-C9A4-4CE9-AAD4-D48B4D93F1D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12154,7 +12153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A618C937-D36D-4D02-9DF7-D873BC39888C}" type="CELLRANGE">
+                    <a:fld id="{C7C24F53-C692-4A17-9B3E-8AB31219E5CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12188,7 +12187,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5D9B0D0-3CBC-43D4-AF4D-1B1FB476281F}" type="CELLRANGE">
+                    <a:fld id="{8CB229F4-FD52-4A54-B2F6-A34B55619585}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12222,7 +12221,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEF65535-89DD-458A-93E1-2180894A5D19}" type="CELLRANGE">
+                    <a:fld id="{365613FD-9CF1-4518-AD08-F1DD7043D0E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12256,7 +12255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFCE64D6-D321-4576-816F-E5E471ECE549}" type="CELLRANGE">
+                    <a:fld id="{AA53F5D0-9F85-4DFD-963D-0B8A192D7A36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12290,7 +12289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{986AB968-3371-41A1-9DBA-296647291137}" type="CELLRANGE">
+                    <a:fld id="{B2CD5892-282D-4D55-B64B-696CE3140FAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12324,7 +12323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9938ABEA-258D-45DF-936E-2751D5CA880C}" type="CELLRANGE">
+                    <a:fld id="{8AD86803-6A59-4335-99B8-7AAA9ACD99D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12358,7 +12357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70F1025F-C953-476F-84D0-8C063A732BC5}" type="CELLRANGE">
+                    <a:fld id="{D88E1656-03C8-46F4-AF34-76684DB8687D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12392,7 +12391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{080065CE-5883-44B6-8B6B-E8BFFF087B65}" type="CELLRANGE">
+                    <a:fld id="{47BB4DC8-25EB-4CA0-ADE9-789F7F31EEA4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12426,7 +12425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A7F494B-8E1D-439F-B52A-3FCAE7D87DCC}" type="CELLRANGE">
+                    <a:fld id="{F5C34759-B3B2-4228-8B6F-30B4148D16C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12460,7 +12459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C63B00D-8B8F-45A5-B76A-81F8870232B7}" type="CELLRANGE">
+                    <a:fld id="{E8197F3B-FB36-463B-9FAA-1D42E11688D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12494,7 +12493,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75A05ADD-E351-49BB-A686-E23EA2351D9C}" type="CELLRANGE">
+                    <a:fld id="{5BE8261F-B1BA-423E-8C01-3BBDDB1BDDD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12528,7 +12527,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6ACEE67C-E3BA-4154-B310-0E1180B8C8A3}" type="CELLRANGE">
+                    <a:fld id="{C7118175-265B-4DBB-B342-129771486C70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12562,7 +12561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{990526FB-721F-4A5E-9182-A3F1BC7741BF}" type="CELLRANGE">
+                    <a:fld id="{EC9A6725-DAAD-4B50-AB18-36AD2246E044}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12596,7 +12595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80CF5C89-8C77-4D03-986E-DB53E26692A6}" type="CELLRANGE">
+                    <a:fld id="{DC94D7C6-5A0B-4408-825E-EC83D06A0758}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12630,7 +12629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D23EA5C-A8A9-4447-B2AC-7575E4DEDFE0}" type="CELLRANGE">
+                    <a:fld id="{4EC60DFC-EDED-4E34-9D6F-282A2568CBA4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12664,7 +12663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8D1BBF0-B2BD-4E54-91AD-C0E03E38D08E}" type="CELLRANGE">
+                    <a:fld id="{C97E2209-3924-4005-8515-5FF049D025D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12698,7 +12697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DC86EB8-A078-4540-A32E-F439E036292F}" type="CELLRANGE">
+                    <a:fld id="{2CDD0767-C1B0-4EC2-9CA1-493FDF87C33B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12732,7 +12731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85DD9708-2407-4AF2-831D-8F2E94DD2CD1}" type="CELLRANGE">
+                    <a:fld id="{42A26CE8-8EAF-446B-8C22-6E10088BF87D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12766,7 +12765,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{023BC288-33F4-4255-84E3-FBCD9DED08A6}" type="CELLRANGE">
+                    <a:fld id="{492FF094-4E37-4FE2-B8DE-CF0B1A394092}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12800,7 +12799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99EE3F46-AF2E-48A1-AD3F-C3355B76B8F1}" type="CELLRANGE">
+                    <a:fld id="{36DB5280-AAED-4282-92BA-3A3790B5D379}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12834,7 +12833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{421624F5-2256-4C68-8FBA-A40853EE908D}" type="CELLRANGE">
+                    <a:fld id="{C7E83D9E-8AD0-4491-AB25-2C1624C14134}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12868,7 +12867,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34FCF639-7243-433F-A6A0-F6B5DA94B94D}" type="CELLRANGE">
+                    <a:fld id="{80022170-F3A6-446A-8AFB-562B3A95528D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12902,7 +12901,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9987FD9-247F-4370-BDED-81F59AC0C0CE}" type="CELLRANGE">
+                    <a:fld id="{BF85FDDA-1492-48F5-B3F9-59E6E8F472AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12936,7 +12935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BC5A0A5-153A-46A7-BD4D-708EEA7F5DDC}" type="CELLRANGE">
+                    <a:fld id="{4173BD76-5D35-438F-8851-62073B1DB08B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12970,7 +12969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0EECCAF-480F-4822-81AA-50EE29D82D0F}" type="CELLRANGE">
+                    <a:fld id="{C0C2C528-92E5-416C-B72E-902A1D24555B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13004,7 +13003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FB4315F-4EE5-43E7-B43F-7BD806382A80}" type="CELLRANGE">
+                    <a:fld id="{36B7F356-4E87-44F4-8C15-7EC62041B338}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13038,7 +13037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D04B8D6A-D360-492E-97AE-FB88D389A655}" type="CELLRANGE">
+                    <a:fld id="{096E23B2-4D41-4199-B7C7-B1AF3BA2E613}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13072,7 +13071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9267CDEC-8A17-4D27-A3B5-064EC34E0B83}" type="CELLRANGE">
+                    <a:fld id="{27CAE512-9504-40E1-A6CE-8AA1036C9EE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13106,7 +13105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65D3FF74-0005-4708-8597-BF284C0B4D44}" type="CELLRANGE">
+                    <a:fld id="{B0179C8C-FB31-4772-B933-A9550F157F97}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13140,7 +13139,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{983891C9-F065-449C-901D-B010DC35700C}" type="CELLRANGE">
+                    <a:fld id="{CFA28765-8583-46CD-9D00-78B945463B6C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13174,7 +13173,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EEF3A4C-A3AA-4567-B5F5-9403D06BE7EC}" type="CELLRANGE">
+                    <a:fld id="{3B955A70-988C-4675-B602-8D6447F8BD8D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13208,7 +13207,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2228468-958F-4BF1-8906-9BEF4835573C}" type="CELLRANGE">
+                    <a:fld id="{D5951627-7634-43AC-BD2A-1BF2EBBE7C74}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13242,7 +13241,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AA93382-A4BB-4840-8613-3AA627465175}" type="CELLRANGE">
+                    <a:fld id="{56437854-7C28-4CC4-9A8F-05A1B465FB18}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13276,7 +13275,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9BC8356-BD67-46EC-A30E-0B7363A03280}" type="CELLRANGE">
+                    <a:fld id="{9B557003-858A-4329-A724-025E3FEE36CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13310,7 +13309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29E970C8-878E-42A5-88B6-7E16FCD30C3B}" type="CELLRANGE">
+                    <a:fld id="{108EAFF2-66E6-42B1-830F-59E04F66AD31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13344,7 +13343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{616BD273-1C5B-4903-AFE9-16BB26C543CC}" type="CELLRANGE">
+                    <a:fld id="{CBF1766E-17AF-415E-9D0D-BAB25538D2EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13378,7 +13377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CD8080A-484C-4A53-A5BF-1C3F8154ED9F}" type="CELLRANGE">
+                    <a:fld id="{4662CE35-60CD-4DB6-9563-72E832BBC2D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13412,7 +13411,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7D595BA-E1E7-4D5E-A173-B25EB295C961}" type="CELLRANGE">
+                    <a:fld id="{BDBB043B-53E2-4D3C-B097-448F52BA0768}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13446,7 +13445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90610741-6E01-4D4E-91C1-EC6B1A1BF7B5}" type="CELLRANGE">
+                    <a:fld id="{86F2DE34-B8C3-4812-A0C1-0008DFEA0EBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13480,7 +13479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E7E4E59-0DF1-44B9-9353-160948BDB287}" type="CELLRANGE">
+                    <a:fld id="{10A5F32A-1E34-43F0-B308-00A9A7E3885E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13514,7 +13513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95CFFE26-F911-444B-8A86-AA3684865034}" type="CELLRANGE">
+                    <a:fld id="{BDC98BF2-1F1D-4EF7-A696-99A8E61DD546}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13548,7 +13547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22153B17-CB89-4517-8E58-5438CE267790}" type="CELLRANGE">
+                    <a:fld id="{5F71F85E-C547-4386-9C2D-5AD524E388CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13582,7 +13581,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDD4A6AE-4A70-4059-831C-9EE124C0938A}" type="CELLRANGE">
+                    <a:fld id="{21AEE1B0-8775-4B5B-A399-834AC9A195C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13616,7 +13615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D673742-112E-4C8B-861D-8CB6907D7DA5}" type="CELLRANGE">
+                    <a:fld id="{F2423B95-D271-43E2-8EE1-33126477C44B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13650,7 +13649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4B672AE-6843-4D73-A79B-FBE958A6CE56}" type="CELLRANGE">
+                    <a:fld id="{385CFD9C-B496-47CB-9E13-DDEFB03C2C53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13684,7 +13683,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AAE0711-3CDB-4F2E-88A7-0E0AB4F64606}" type="CELLRANGE">
+                    <a:fld id="{DD100825-1A4B-4541-897F-938D19BBB106}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13718,7 +13717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81F3FF1B-3705-4CE4-99A6-8676A46190EC}" type="CELLRANGE">
+                    <a:fld id="{B85E3A86-E41D-4853-B4A9-001DAC3E7A85}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14848,7 +14847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34365852-48D8-419C-A09A-C9DE01981F7A}" type="CELLRANGE">
+                    <a:fld id="{99B1889C-3AFF-4FAF-960C-C4418054C2F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14882,7 +14881,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4A8AE5D-09A7-4790-A6D5-5116777495D0}" type="CELLRANGE">
+                    <a:fld id="{A36ED4F6-AB6E-428B-9237-44ED01D61334}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14916,7 +14915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76C4E2CD-A25A-41F2-B464-0E8D68EEAE75}" type="CELLRANGE">
+                    <a:fld id="{52136295-F351-4F55-B1E4-BBCEF235492E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14950,7 +14949,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7954A837-1584-4222-A81C-60137806A65B}" type="CELLRANGE">
+                    <a:fld id="{4A760011-A097-48E2-858A-99FCC9351917}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14984,7 +14983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5D83DEF-F2EB-45F5-94DF-2E095438AF71}" type="CELLRANGE">
+                    <a:fld id="{0409B67E-C375-4FD2-9682-621FEDA393B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15018,7 +15017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{893F9A12-39EE-432B-B55E-3F7E9BF8B230}" type="CELLRANGE">
+                    <a:fld id="{94E4BA52-71D9-4A18-8FB3-D787BAFD3EA0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15052,7 +15051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0BA199D-73F5-4C59-9D08-65233590C10D}" type="CELLRANGE">
+                    <a:fld id="{8DCD2386-409F-4B68-982C-ECCB976FF245}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15086,7 +15085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3709F72F-FD87-4926-8733-DF31776B1D25}" type="CELLRANGE">
+                    <a:fld id="{1802DE3F-1E2F-47B6-996A-B007FA4C6B1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15120,7 +15119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A8A9AA1-634A-489F-A1E7-E704DC720912}" type="CELLRANGE">
+                    <a:fld id="{300DE3B7-EECB-4AA8-81CD-535E29A97136}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15154,7 +15153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19A351BB-1AEE-4E39-A4F3-01AE59E310FE}" type="CELLRANGE">
+                    <a:fld id="{F189DEB1-DF03-45ED-8E80-0C4654984360}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15188,7 +15187,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B538CE7D-EA5C-46B0-A148-A0573D9ABFA8}" type="CELLRANGE">
+                    <a:fld id="{5201E0BA-C528-457E-A3DB-34657A1FDCB5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15222,7 +15221,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42490B51-54C2-4014-BD44-07E91599F780}" type="CELLRANGE">
+                    <a:fld id="{6CE9AC47-26AC-4D3B-8446-D8DA788D52F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15256,7 +15255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09AAF28B-BA76-4EBB-BD0D-6AA9B8A805A0}" type="CELLRANGE">
+                    <a:fld id="{D10A8BAE-96DE-45B4-B86E-BAEC83AE837F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15290,7 +15289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D5DBD00-98A2-4238-BAA5-E7354B4F635E}" type="CELLRANGE">
+                    <a:fld id="{C3613413-A086-43E0-B48F-D30AA763D5D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15324,7 +15323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5599F34-B89A-46CC-A6EA-62F2A7FEC609}" type="CELLRANGE">
+                    <a:fld id="{536C717C-C36C-449C-85AF-CAA2CD7C7AE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15358,7 +15357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{567F1D5F-F1BE-440F-8EDD-37D96E4A9E38}" type="CELLRANGE">
+                    <a:fld id="{C82DE563-0CE5-4F65-A5C2-4ED1526CECBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15392,7 +15391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AAC2FF0-87EF-4D00-AA06-A771444799C4}" type="CELLRANGE">
+                    <a:fld id="{EDA5DF62-00BA-46D6-82E8-D52F6123CD0D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15426,7 +15425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F39DA4C5-6A22-4F6C-9B7F-1DCC17DEEF87}" type="CELLRANGE">
+                    <a:fld id="{ED7994D9-976A-467F-815D-C85B9BDEB83B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15460,7 +15459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81C8B65F-5673-4094-86E9-C2C681A3C457}" type="CELLRANGE">
+                    <a:fld id="{7F3A117C-7ED5-41E8-8825-8756879F21EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15494,7 +15493,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{618E2CA6-68BE-4721-97F6-4E1A73D04F07}" type="CELLRANGE">
+                    <a:fld id="{65ABDB17-2DDF-4CFD-AF54-25B0B41BE7B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15528,7 +15527,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F68070CE-2D96-4ED4-8D26-7CC3FC82EAEB}" type="CELLRANGE">
+                    <a:fld id="{43968CCA-1715-498E-8988-4699DF4DBA26}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15562,7 +15561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D18E2A78-5F90-4C5C-84B2-F1C1F7B7AD88}" type="CELLRANGE">
+                    <a:fld id="{EB0AA0C5-EDCA-4C7A-B448-AB0E975AF7F7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15596,7 +15595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AB9CED7-8EA2-4B68-A958-6111DCB8D2B6}" type="CELLRANGE">
+                    <a:fld id="{00452A1E-A8C5-497B-826D-EA7F41524548}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15630,7 +15629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A0852EC-B2D1-4EE9-8358-C0676DBDC0E4}" type="CELLRANGE">
+                    <a:fld id="{362EE86D-B1B2-4876-A33F-34FFC997E1C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15664,7 +15663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D31FFA2B-8EA8-4331-9798-BEF0EEF3D6DE}" type="CELLRANGE">
+                    <a:fld id="{42BBADF8-5EFC-4249-896C-7BE05EF62AD1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15698,7 +15697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2FA8F0A-6513-4CE2-8E3F-498AB6658B35}" type="CELLRANGE">
+                    <a:fld id="{FD4E1C6C-519A-4508-BCE5-FF8745797228}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15732,7 +15731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91B2202E-B33D-4031-B93C-B41F3486A097}" type="CELLRANGE">
+                    <a:fld id="{6AF31FD8-B56D-44B4-9FD1-160E494C4C3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15766,7 +15765,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB32D6B7-E599-4F86-8317-3D0F173B1FBF}" type="CELLRANGE">
+                    <a:fld id="{093D6206-B0AB-456E-AF8E-B6C0B7D3F939}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15800,7 +15799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4051184-4DFA-4917-AA1E-3D4DDF6E3A52}" type="CELLRANGE">
+                    <a:fld id="{29249B5E-62AD-4E4D-87F7-372AE4938941}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15834,7 +15833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CE2EBEA-B49E-4057-BD2C-022AEE89B3B3}" type="CELLRANGE">
+                    <a:fld id="{2700EDEF-4F66-4C9F-8EA5-18814B3F31B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15868,7 +15867,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEF5819D-A8DF-4B13-9228-927DE9F02A2C}" type="CELLRANGE">
+                    <a:fld id="{CBE4F751-3BFB-459B-8612-FB97F51B981A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15902,7 +15901,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0453B9E-9362-44D8-AF0A-71236A95A0AF}" type="CELLRANGE">
+                    <a:fld id="{798903F2-2FF6-438C-928E-3FB9A9B0C8BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15936,7 +15935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{173596E7-ECE5-4834-8A5E-F82A6F2281E4}" type="CELLRANGE">
+                    <a:fld id="{81A555A6-4FC3-4E7F-AA5F-86B56E171FA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -15970,7 +15969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B949A440-50C9-4E82-B955-7A64EB9DFC86}" type="CELLRANGE">
+                    <a:fld id="{B47F268A-DA6C-4FDA-B760-8039D36BB3C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16004,7 +16003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2681329A-89FE-4C83-A86C-1DAA347A2F55}" type="CELLRANGE">
+                    <a:fld id="{4CB9FCC6-7797-4480-9D28-EA560027E41D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16038,7 +16037,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE7964D4-C72A-46F8-B289-E00FD44DF3AB}" type="CELLRANGE">
+                    <a:fld id="{AA8B7BF2-1992-4354-8175-47E13C991A0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16072,7 +16071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AD74C32-6821-4C88-861D-04D37953C7D3}" type="CELLRANGE">
+                    <a:fld id="{C682489B-42F3-4FAA-BCC5-51578A64DFB6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16106,7 +16105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C2E408C-C260-4266-9C85-6AC2CA7E6685}" type="CELLRANGE">
+                    <a:fld id="{45BFD8A7-5D79-481E-9894-7143E11563A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16140,7 +16139,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD25D9A6-6417-4E08-8101-B3253DA65192}" type="CELLRANGE">
+                    <a:fld id="{3632E1D1-2A99-4A39-8383-51A66BF08EBB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16174,7 +16173,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77349B14-0E2A-41FB-B0C4-38FEE47B010C}" type="CELLRANGE">
+                    <a:fld id="{4EA5C6D6-EF47-4A1A-856F-D03ADA6CD53C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16208,7 +16207,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F17600A6-72F1-46FE-B6AC-2B87D8D83E54}" type="CELLRANGE">
+                    <a:fld id="{122875BA-68B1-4DC7-9A05-E4D4D8571F20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16242,7 +16241,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{302F5DCF-C2B4-4218-AC2F-4B49E33D958C}" type="CELLRANGE">
+                    <a:fld id="{DADDD6F3-9351-4973-AB2B-24AD98863F44}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16276,7 +16275,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CAE77CC-5567-40D0-82AB-069F8688FCE0}" type="CELLRANGE">
+                    <a:fld id="{AF63ED33-E175-4F04-B473-1172AEF09E41}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16310,7 +16309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43EBDD9F-2EF3-4BFB-9DFF-A90603F9841C}" type="CELLRANGE">
+                    <a:fld id="{BAC5DFB9-A08D-4CCD-89C2-9DF97D8CD32E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16344,7 +16343,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65F844E2-8526-4F9A-B07E-3DC1AA87391E}" type="CELLRANGE">
+                    <a:fld id="{E49C3F1C-3978-41C1-A7CC-2E15D0758E25}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16378,7 +16377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{659CF07A-6A66-41CD-95E0-95AC19762164}" type="CELLRANGE">
+                    <a:fld id="{EC75FBE1-238F-4E22-B9BF-A4C81B3E5A34}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16412,7 +16411,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35325E28-DF45-4C5C-901F-A0705906C1CC}" type="CELLRANGE">
+                    <a:fld id="{634C5B9A-7BAC-4E66-8AB3-AB200C4A6B65}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16446,7 +16445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFD9155B-68CE-43A6-BACA-A86ECC4D7B69}" type="CELLRANGE">
+                    <a:fld id="{A25772D9-A6F2-4E39-9BA9-EE985B32F837}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16480,7 +16479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D9DC3E2-016A-4EF1-B120-68B700BE992A}" type="CELLRANGE">
+                    <a:fld id="{4CB0BC68-7613-4626-A574-994E851ADAA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16514,7 +16513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4F3AC37-8CD0-4032-AE28-B634DC0B7AD8}" type="CELLRANGE">
+                    <a:fld id="{2EA50019-A5CD-4127-91FD-8ADE485EEFEB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16548,7 +16547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D51A3274-9945-448C-9094-277CF9BAF713}" type="CELLRANGE">
+                    <a:fld id="{FD584C68-BDD3-445C-802A-A73E0CDC3CFF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16582,7 +16581,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DF9D043-389A-435D-A3A5-C4655AAAC496}" type="CELLRANGE">
+                    <a:fld id="{F8C98301-FF03-47AE-9FC3-7E99603B5FDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16616,7 +16615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0257498F-96F5-446F-9DF5-41B32089D4EC}" type="CELLRANGE">
+                    <a:fld id="{694F634A-263C-4B2C-B052-A6B59D4CD24D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16650,7 +16649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3FFAEF9-5ED8-4C89-BF39-2A3470494061}" type="CELLRANGE">
+                    <a:fld id="{55D074E4-8C2F-4709-A173-2927B8F703CC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16684,7 +16683,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{207F7455-FA07-4E4D-98CC-7B7574257E05}" type="CELLRANGE">
+                    <a:fld id="{2DE3E795-2BBF-4757-BEC5-978FC81D87FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16718,7 +16717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48767707-FCEE-41DF-A6A0-567E8B395D57}" type="CELLRANGE">
+                    <a:fld id="{88C03041-D432-4612-A5E0-71957514B914}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16752,7 +16751,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5D09CF4-7D9F-46F4-B9E2-2B33EDF9CE43}" type="CELLRANGE">
+                    <a:fld id="{7C56E59C-DD67-4998-986F-E792F9A8F22C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16786,7 +16785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C842BAEB-5B90-4F4A-A452-A2E765097070}" type="CELLRANGE">
+                    <a:fld id="{82D1193C-EAFC-47B7-88FA-781877D0A0A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16820,7 +16819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B40F68E6-D429-4A8B-90D2-9C79A0238CE8}" type="CELLRANGE">
+                    <a:fld id="{07652AAF-07CF-467C-B0BD-3D436D930A47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16854,7 +16853,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ADBEE8E-C751-453E-8330-3B8E5FD69CFF}" type="CELLRANGE">
+                    <a:fld id="{070A5D1F-0D67-46D0-85C3-014C0421B8BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17983,7 +17982,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19F5EFEB-B01E-4369-B9DF-D907250E608F}" type="CELLRANGE">
+                    <a:fld id="{BB8DDE19-E9A1-41D3-B05A-AA11AA105983}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18017,7 +18016,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4882C6FE-0C74-4CCD-B70B-C14E07747E44}" type="CELLRANGE">
+                    <a:fld id="{A3ED1D11-3BC2-4AE4-9A44-23937429D23F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18051,7 +18050,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C2B0B21-971F-4A09-84B4-BC7AFA1AC798}" type="CELLRANGE">
+                    <a:fld id="{8486E237-383E-48D8-A068-A9A3660F0EF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18085,7 +18084,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD64B2E2-CEDE-45C0-A057-72BE26A86C0A}" type="CELLRANGE">
+                    <a:fld id="{51040089-2847-4438-8CC1-9BE10577B7E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18119,7 +18118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{497B2B62-290D-4D28-872A-F653F7410B6A}" type="CELLRANGE">
+                    <a:fld id="{A43B8282-932D-4787-8058-A39D8E43ACD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18153,7 +18152,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA8AE131-C3D7-42E0-A0A3-6DB39E64B663}" type="CELLRANGE">
+                    <a:fld id="{F8D915C0-B9AE-4A20-A3F9-1B79A91284D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18187,7 +18186,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E311C80-B81E-4F45-9EF3-36C687E7FBFA}" type="CELLRANGE">
+                    <a:fld id="{1740AD7D-0E5D-48E8-8606-072B7B8DC8CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18221,7 +18220,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4311BD22-F840-4D35-89AA-415C4835C321}" type="CELLRANGE">
+                    <a:fld id="{C875A91E-05DE-4422-8AB3-6F8F908B3333}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18255,7 +18254,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DA05D59-773C-4B63-B3BE-DBF06D2496E1}" type="CELLRANGE">
+                    <a:fld id="{6FF669F3-66FA-4DF3-8E6E-AA3E00E4243A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18289,7 +18288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A09F692-7AAB-4305-B8C4-D024FF97C59B}" type="CELLRANGE">
+                    <a:fld id="{0439501F-6798-435D-B440-E321B40557E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18323,7 +18322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1248C68B-80D2-468C-98E7-1A690CCC6559}" type="CELLRANGE">
+                    <a:fld id="{801F655F-98BC-4290-8384-7C27AAE33051}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18357,7 +18356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F30F0C2-71FF-48E3-AB8E-080D0451EE79}" type="CELLRANGE">
+                    <a:fld id="{78888401-E96C-4069-91B9-779A9F1E474D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18391,7 +18390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D61E1F21-4676-456B-81C9-EFF578A5716A}" type="CELLRANGE">
+                    <a:fld id="{9F045BF4-807F-491B-BBBE-97C61CB7DF0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18425,7 +18424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38849419-56BF-4088-9AC8-B094E01406C8}" type="CELLRANGE">
+                    <a:fld id="{670CFBEA-B3FB-4652-9D1C-4AAFCD7EFC12}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18459,7 +18458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAEC70F9-FE3A-442B-991B-2167DC1BCC6E}" type="CELLRANGE">
+                    <a:fld id="{E131DCBA-90FD-4382-A2EB-C1AEA60F6536}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18493,7 +18492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{285E0C50-834B-472B-9A8F-EB712586EF99}" type="CELLRANGE">
+                    <a:fld id="{C0E9906F-36A2-47CC-966A-18225EF324A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18527,7 +18526,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71E2DAAB-40C3-4B48-A709-E8FB0856E1B9}" type="CELLRANGE">
+                    <a:fld id="{96A39E8E-DF1A-46B3-9998-1DE43ED9E71F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18561,7 +18560,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10D29976-09ED-433F-9314-06BDDC92A036}" type="CELLRANGE">
+                    <a:fld id="{DA418F88-9040-4B9D-BF59-335A6579FA6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18595,7 +18594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9017D26C-2AB2-41E5-9EBF-4B5B7EEFDD7A}" type="CELLRANGE">
+                    <a:fld id="{9BFF736E-E244-4498-BCA3-AA010FDB4464}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18629,7 +18628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C2D1ABB-EB75-4C0F-B042-F544201D1906}" type="CELLRANGE">
+                    <a:fld id="{12E21412-6E25-4195-8FE8-39A620A27E5D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18663,7 +18662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{431E5B80-DE25-488F-B9C7-2F495C45B760}" type="CELLRANGE">
+                    <a:fld id="{3ECC8B6E-205E-4CC0-A57C-A849EECA9FFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18697,7 +18696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A89DE8B-C702-4972-BBBC-C780B1590FDB}" type="CELLRANGE">
+                    <a:fld id="{A6C11E0E-FAD4-45BD-87E1-94C1B2138242}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18731,7 +18730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4958EE1A-29B1-4A9D-A2CA-2BA9C8EB5B35}" type="CELLRANGE">
+                    <a:fld id="{0D71A091-303B-4818-A34F-FA881B5798E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18765,7 +18764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E7443EB-C0F4-4D77-ACDB-CFCF32F2DAD4}" type="CELLRANGE">
+                    <a:fld id="{A4E07E79-54D0-47BF-A232-5CB77DBFFE7C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18799,7 +18798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{732B104B-6AD9-4DD7-818F-10B0BC4F10C3}" type="CELLRANGE">
+                    <a:fld id="{51F50C5F-B0DA-40FE-ABA4-F338FB233E2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18833,7 +18832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9D64B88-9C45-4D95-8A86-812C4807DB76}" type="CELLRANGE">
+                    <a:fld id="{53547F64-A614-443B-99DE-06C073E004C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18867,7 +18866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBAE0E89-4E0A-451C-A36B-6C2965926447}" type="CELLRANGE">
+                    <a:fld id="{0090DDEE-68E1-4D78-A585-2B7F956059BB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18901,7 +18900,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF26AD9A-A78B-47EE-970C-DD6DD4AA1087}" type="CELLRANGE">
+                    <a:fld id="{4FC6B445-74F1-4348-962E-76017D4EBA1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18935,7 +18934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B95F321-6D25-4AA6-ABB1-4B77A7D7173E}" type="CELLRANGE">
+                    <a:fld id="{BB85DB3D-8D4D-4EDD-B730-2D254FD54E99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18969,7 +18968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C2CB92AE-2EC1-442A-BD12-AE0B375C4487}" type="CELLRANGE">
+                    <a:fld id="{BEB2DE29-0459-4DED-9A39-657200B1CF89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19003,7 +19002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25213C81-4EC1-4841-91C5-7A9C82753F77}" type="CELLRANGE">
+                    <a:fld id="{581651BD-862E-4C6C-8BAF-4CC085B352F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19037,7 +19036,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA6CD739-5191-4068-A86A-0EB86C36058C}" type="CELLRANGE">
+                    <a:fld id="{6EF5F712-8CDC-4ACC-BBE3-110B532A1DA9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19071,7 +19070,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{447BACC6-B21A-4A60-9D8B-71B36D4194B3}" type="CELLRANGE">
+                    <a:fld id="{4BF23041-B0AF-44C0-AA8F-17CB754705D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19105,7 +19104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12547DB2-BA59-42C6-A0D9-33C8D2F0C0ED}" type="CELLRANGE">
+                    <a:fld id="{7664335C-C5D5-46C2-8258-99BB648C06E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19139,7 +19138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67A2EE09-9AFF-4C40-A2FA-BE251617A91C}" type="CELLRANGE">
+                    <a:fld id="{95BC2595-8045-46F6-B4B5-BBE6911F9952}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19173,7 +19172,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6409AD80-AA34-4B5C-A306-6A3DA8253335}" type="CELLRANGE">
+                    <a:fld id="{BA1076B5-7AAC-48A0-AE66-5F3E64A91166}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19207,7 +19206,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5960437-3425-4608-BA92-BE91931467B9}" type="CELLRANGE">
+                    <a:fld id="{CB5F226C-3A94-4488-9F8F-29C86CA07404}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19241,7 +19240,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C68DA13-4887-4129-9288-4773C0725A9E}" type="CELLRANGE">
+                    <a:fld id="{F0AD58D4-6C12-4337-8452-4D6712784F16}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19275,7 +19274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5DD8716-10FA-42A3-8B07-FD3F99A42BFC}" type="CELLRANGE">
+                    <a:fld id="{99540149-D14E-4375-A340-A75451B3A0A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19309,7 +19308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F21B530-9B51-4EDF-B129-AC353B8B9A60}" type="CELLRANGE">
+                    <a:fld id="{9E12A3C4-E29D-4343-8405-9D55CFBA9BA7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19343,7 +19342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9EE23A2-387B-4FE6-B115-47374C80269A}" type="CELLRANGE">
+                    <a:fld id="{2E01D9C3-F53F-4AB4-9CED-13211680E4A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19377,7 +19376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69A4F35E-821E-4A91-947A-875C842C1917}" type="CELLRANGE">
+                    <a:fld id="{972EC5E6-4141-48B7-8BAF-3F4D358FED9C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19411,7 +19410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{483AEB77-6F8F-4EBE-BA9A-0B7FF1C89964}" type="CELLRANGE">
+                    <a:fld id="{8B3494F4-E3C2-4087-96AE-FCBF93CC09AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19445,7 +19444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB075FA7-E014-460B-A91A-D42B82CE68D4}" type="CELLRANGE">
+                    <a:fld id="{459C2C29-FD38-48D3-A106-C3044ADECFF1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19479,7 +19478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F5F8E9E-C3E2-4748-A814-0B1B92F0B8B0}" type="CELLRANGE">
+                    <a:fld id="{4719251F-DFF1-4373-8D0A-565E0A0E0E90}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19513,7 +19512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE693941-671A-4C4C-AFB3-8C365B02D248}" type="CELLRANGE">
+                    <a:fld id="{4BA56940-A495-4617-B221-1CBF78ABEDC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19547,7 +19546,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C862FBA-ADF4-4FA1-9D08-55FEED5755A0}" type="CELLRANGE">
+                    <a:fld id="{B5155F3D-71D2-4B69-A07D-F477777B91DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19581,7 +19580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42EB0EFC-2750-4D4C-9CCB-B31615AA6972}" type="CELLRANGE">
+                    <a:fld id="{62B7E1E4-FBAF-402E-B9E4-6BBB108AFF7C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19615,7 +19614,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AEB3F92A-FB6C-445E-AD56-FFCE495B6AEF}" type="CELLRANGE">
+                    <a:fld id="{AF21AB89-7954-4E11-BE0E-7D36613C41D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19649,7 +19648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8F9DBC9-D0B0-4576-8E05-0E2E2B5782DC}" type="CELLRANGE">
+                    <a:fld id="{8E212BC3-CA6A-45EC-87C2-DC62054F2337}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19683,7 +19682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E6CF050-1D9B-4CB2-8EB1-97F88231202F}" type="CELLRANGE">
+                    <a:fld id="{D14A6406-1D21-4847-9288-1EA53C1E7DD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19717,7 +19716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F556F4D3-C5DD-451C-8E72-9A3EEC358111}" type="CELLRANGE">
+                    <a:fld id="{137ABE7E-4B72-47C1-94E0-DF2500FF65A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19751,7 +19750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C25D4E8-F13B-4EA0-88E9-CA6D05DC6CC2}" type="CELLRANGE">
+                    <a:fld id="{7D458CD2-3A96-4C29-8567-227DF62A3906}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19785,7 +19784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24208EA9-1CFF-4C6E-A6AC-95ABC675586D}" type="CELLRANGE">
+                    <a:fld id="{3C3E0380-F289-441B-B767-F88526C2814E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19819,7 +19818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1995D79-BA3D-4A05-84D4-9980C63CA9B3}" type="CELLRANGE">
+                    <a:fld id="{8D2CB259-DC7A-434A-BD44-EAD5CCC91392}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19853,7 +19852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6488220C-FC98-41CE-86BD-645347F5842A}" type="CELLRANGE">
+                    <a:fld id="{6C1D0563-7540-43F3-B86F-2B41EEE84FA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19887,7 +19886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF02B5D7-3E98-48E7-93FF-51DA8F5ADD8C}" type="CELLRANGE">
+                    <a:fld id="{A62B90C7-3A89-4B13-8758-F5540470153C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19921,7 +19920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E9D0729-184F-411D-A4B4-A3E0777900A4}" type="CELLRANGE">
+                    <a:fld id="{F93AD5BC-2AA6-4AB2-B734-3035468346B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19955,7 +19954,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7686753D-A096-4256-9F7E-9C0A8008D78F}" type="CELLRANGE">
+                    <a:fld id="{3639BBB8-70D9-48D1-8237-BB317EF32958}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19989,7 +19988,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43DE4799-D158-4E43-9563-05CACD9019C7}" type="CELLRANGE">
+                    <a:fld id="{8A8B5A22-5FC6-4BFB-B97F-3C7BC9A1D9F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21118,7 +21117,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87C38B31-F3B2-460E-80E5-AF46AD33C0A7}" type="CELLRANGE">
+                    <a:fld id="{CD4CF5B9-10E2-474E-BB33-CCBAEBA8475B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21152,7 +21151,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B092AD1-9030-45E6-A2B0-7D20BCF68FBE}" type="CELLRANGE">
+                    <a:fld id="{A5F5C20A-C861-4227-A0CD-698AD6EEC39B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21186,7 +21185,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9119F5FC-6614-4A98-90A9-1B8F7AF65463}" type="CELLRANGE">
+                    <a:fld id="{0E267AA1-D1F0-467C-8EAC-EEFE45830A76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21220,7 +21219,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{347AB941-4A9E-4D56-8302-DD69ED3FA69B}" type="CELLRANGE">
+                    <a:fld id="{54A0355F-C59C-428A-A809-FABC489EA609}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21254,7 +21253,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96920D93-DEEA-49A7-B555-93E7249B391B}" type="CELLRANGE">
+                    <a:fld id="{98878B59-7AC3-4588-8ED6-50835AB68522}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21288,7 +21287,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A70FE1F9-A3E0-4BFE-A32C-E8FC15A54725}" type="CELLRANGE">
+                    <a:fld id="{F891AC7F-2C00-4138-AD3E-19C021A6BA7E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21322,7 +21321,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8FC1B051-6B4E-4ECD-B049-FEB98AD8CD74}" type="CELLRANGE">
+                    <a:fld id="{BEC1E0D6-8AFF-4CD6-98BB-6756E8AE20D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21356,7 +21355,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D160F28-1CA8-451E-AE0B-55525F641C25}" type="CELLRANGE">
+                    <a:fld id="{70BBC2DE-0107-4B11-BEFF-88BC7DB640A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21390,7 +21389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94F0D27F-52D5-48A3-8246-9916380F1388}" type="CELLRANGE">
+                    <a:fld id="{8C74EF17-7F45-46E3-88C0-328F4DAF379D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21424,7 +21423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54090056-F75A-4702-BD72-3EE9451E9301}" type="CELLRANGE">
+                    <a:fld id="{2D08B833-0C7C-40B6-BF34-600EDA05F5D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21458,7 +21457,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8759AB19-02B5-4F41-900B-01B254FF34B2}" type="CELLRANGE">
+                    <a:fld id="{45561195-DE3D-4E27-8D80-32EF977837BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21492,7 +21491,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10D397A0-583A-4588-908C-52AD5BF3AF3E}" type="CELLRANGE">
+                    <a:fld id="{05DD000E-8DF2-4440-819A-74B2DDE409AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21526,7 +21525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16333EFB-1D98-4435-8250-3720E0622224}" type="CELLRANGE">
+                    <a:fld id="{B1338032-8767-48E0-8BCE-606AFA35B715}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21560,7 +21559,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{389B5E8C-FFAB-44E6-B1F4-7B5AF6648D8B}" type="CELLRANGE">
+                    <a:fld id="{D1248CA3-E963-448E-9234-72EC6D3291A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21594,7 +21593,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5774F2E-24E0-4269-A4E0-C0220EB82407}" type="CELLRANGE">
+                    <a:fld id="{C140CB6D-E3F2-4EF4-8A6F-94A45478300B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21628,7 +21627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36BE42F4-3075-4777-A9CE-7DB0E3AECB16}" type="CELLRANGE">
+                    <a:fld id="{32769A82-4FF1-4798-A590-E1C89490C0E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21662,7 +21661,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F60B756-9840-4887-8858-988254CCEC09}" type="CELLRANGE">
+                    <a:fld id="{EDFAF25A-4865-4781-87D0-E7F68B29654B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21696,7 +21695,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D680E566-126C-4906-8811-835B6C56DEC7}" type="CELLRANGE">
+                    <a:fld id="{98D1E5D8-50E1-439D-BAA0-5465D60686F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21730,7 +21729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E83E969-E936-43FB-9436-7C90B2EBD9EB}" type="CELLRANGE">
+                    <a:fld id="{8FE53821-2B9C-44E7-BCA9-C7DB257A1BD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21764,7 +21763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D3BF448-A03A-45A0-A331-2F7171F0C67F}" type="CELLRANGE">
+                    <a:fld id="{AFB849B7-8CD2-424E-A7B5-FAD7DF3F818D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21798,7 +21797,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{257C5479-7272-4F5C-A5B1-27D0AD779BBE}" type="CELLRANGE">
+                    <a:fld id="{24F9E0CD-B647-4254-BD3C-D303E30A0516}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21832,7 +21831,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9F1CFDB-75F9-459C-8D46-3C600B0CACDB}" type="CELLRANGE">
+                    <a:fld id="{C3A72EC4-BBB3-41B1-B0CF-F5B1677CEA8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21866,7 +21865,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C36D604B-64BD-4EA0-9A48-8F42731161E7}" type="CELLRANGE">
+                    <a:fld id="{881F20FB-B4AA-4E66-8DCF-6E70A4439693}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21900,7 +21899,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{235F16B5-FFF7-483D-8A71-7166B8357C62}" type="CELLRANGE">
+                    <a:fld id="{F496BD8D-B48C-48F0-BB76-AC83679FF701}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21934,7 +21933,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F591A868-B996-4839-B8ED-44094D5E7CDB}" type="CELLRANGE">
+                    <a:fld id="{5B8C34C1-E2E0-4372-80CF-E533F05F6670}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -21968,7 +21967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8321B07F-E347-4964-B69F-14D8B5579E1E}" type="CELLRANGE">
+                    <a:fld id="{527FC060-084F-466D-AE70-2F844987F044}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22002,7 +22001,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DCFCDFB-1BD7-4B88-BEFA-F653F9CD7570}" type="CELLRANGE">
+                    <a:fld id="{3E863756-1846-4E50-AEA0-B15B8E65B1D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22036,7 +22035,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47B3A801-5284-469D-8114-C4999D85C4B3}" type="CELLRANGE">
+                    <a:fld id="{F533A360-C7A6-4812-B850-66C2E4A7425D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22070,7 +22069,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DDD608F-796B-4A61-8754-0C807DE4F655}" type="CELLRANGE">
+                    <a:fld id="{B5BC24C9-3D81-48C7-8909-463E9F694741}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22104,7 +22103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFFE7025-B9A7-4C07-AA6E-33E7C8EF4C85}" type="CELLRANGE">
+                    <a:fld id="{BCA35BD6-B59E-47A0-B18A-CDCB06641C2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22138,7 +22137,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C1802FE-5667-447D-9384-4BAC924D9CDA}" type="CELLRANGE">
+                    <a:fld id="{CD2A7751-B776-463F-8C3B-9E36E82098F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22172,7 +22171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7D63620-EDA0-4707-9CEE-6547EE77778D}" type="CELLRANGE">
+                    <a:fld id="{ADE00D18-B627-405A-8EEE-ABD72DBCB7A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22206,7 +22205,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56A4D6BB-9BA1-45F3-BD2C-D5EAB610CEA3}" type="CELLRANGE">
+                    <a:fld id="{707722A2-2245-454A-AE9B-DB0238898D5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22240,7 +22239,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1030FC61-4272-43C4-A0DB-DA66BA4A65E7}" type="CELLRANGE">
+                    <a:fld id="{222DA0E2-26E6-4A74-891E-70DFBCA2906D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22274,7 +22273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C980B1EA-58BE-43A5-803E-E5228A74F364}" type="CELLRANGE">
+                    <a:fld id="{A66C318C-58FA-4104-B541-B35B40A84C7D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22308,7 +22307,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DB23B0A-E181-4DDC-B277-9BB8132329A1}" type="CELLRANGE">
+                    <a:fld id="{94CCF816-2DE7-4F6E-BCF0-51C1DC364C70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22342,7 +22341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89967B9E-962A-4B43-96C9-0716F1A621BC}" type="CELLRANGE">
+                    <a:fld id="{77C3CDED-59DE-451F-BCFB-7072A19C9C93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22376,7 +22375,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5873B5DA-D3FA-466D-9D32-B0A619C6EF4D}" type="CELLRANGE">
+                    <a:fld id="{04334F99-B057-48E0-B74C-DD83A5A4F82F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22410,7 +22409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D496935A-8CD1-4E20-BDCE-B7B8ED1E7A72}" type="CELLRANGE">
+                    <a:fld id="{510A7485-C910-4275-AD7A-76EC08471A9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22444,7 +22443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BA636FE-87F8-4BA2-ACCB-0982ADD2C498}" type="CELLRANGE">
+                    <a:fld id="{CABD10D2-E280-46BC-AE05-39106508CFD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22478,7 +22477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C7E3F31-DA31-4D4B-99F6-0D27162DB495}" type="CELLRANGE">
+                    <a:fld id="{D1A58ADA-4C14-4032-9CD3-B79964BCF581}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22512,7 +22511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58139147-0FEF-48C0-9C13-BD4880735E0B}" type="CELLRANGE">
+                    <a:fld id="{4CF0B1B3-724B-4379-A2BD-5376F3A259AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22546,7 +22545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0B9DEDA-131C-4020-9707-16E4CC345E92}" type="CELLRANGE">
+                    <a:fld id="{DFBE97AF-8D70-410A-912A-01213BAB001B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22580,7 +22579,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE36D7E5-FD7F-4AC9-AC65-C29A71967585}" type="CELLRANGE">
+                    <a:fld id="{8F57BCE1-FA68-4598-A0CE-980CB51276FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22614,7 +22613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{212076F1-4864-4D96-9003-F24152B88C25}" type="CELLRANGE">
+                    <a:fld id="{E80043F3-A45D-4E87-B7C7-462655D2C387}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22648,7 +22647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7CB257D-6A44-4F61-996E-25D39F3C1588}" type="CELLRANGE">
+                    <a:fld id="{6BA3F212-D38F-4318-ABC8-A9FD5C91236C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22682,7 +22681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A98588EB-5335-4AC5-B074-3CF7C8C350A3}" type="CELLRANGE">
+                    <a:fld id="{E24EBB23-E425-426E-ADD0-EF181277EB0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22716,7 +22715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63804F65-FCA2-44C6-89CE-34D8B27D439B}" type="CELLRANGE">
+                    <a:fld id="{C7436FBF-A2F7-49DC-8B83-04B636DAA670}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22750,7 +22749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{533F7EA9-3F35-4C82-81D2-0BBBC81FE568}" type="CELLRANGE">
+                    <a:fld id="{A9DE7AFA-E76D-49F3-BE24-0F87E738CC9F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22784,7 +22783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D769C2D4-0529-49C8-B804-BE45B707B7E0}" type="CELLRANGE">
+                    <a:fld id="{1634024E-7F81-4232-8467-6D8299DF8082}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22818,7 +22817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7378973-1C80-449B-8AD2-F4ACC02E4724}" type="CELLRANGE">
+                    <a:fld id="{89C66C7D-C6BE-4A6B-B5B5-1611CF22EA1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22852,7 +22851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47D5BEC3-27EC-47D4-9CD7-E0203BCFABA7}" type="CELLRANGE">
+                    <a:fld id="{8B929171-931C-4A2C-83CC-06EEA9368762}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22886,7 +22885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1DFC05F2-8112-4B92-A25A-51F3C21D6AE9}" type="CELLRANGE">
+                    <a:fld id="{2368B6B2-ECFE-48FE-A8FD-74D5541C2557}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22920,7 +22919,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCD211AC-452C-41B5-B738-0DD55E4E5452}" type="CELLRANGE">
+                    <a:fld id="{CE07F999-6B85-4F2B-A0CB-FB1D0BA120EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22954,7 +22953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C77A8FD3-AD94-4284-BA24-E74681B5E3F0}" type="CELLRANGE">
+                    <a:fld id="{A88CB15C-6B8D-4860-A93A-9E0EA5BBD105}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -22988,7 +22987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B19190E-2F8C-47C8-A3D9-CFB988593C3D}" type="CELLRANGE">
+                    <a:fld id="{C796AD2D-F951-45B6-AF85-23AAD1835048}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -23022,7 +23021,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4160E53-75D8-4955-BAE1-DD2E6E1292C9}" type="CELLRANGE">
+                    <a:fld id="{A693B949-4CE7-4870-92A3-6777E82885E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -23056,7 +23055,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACCBFC2D-B593-42BC-9DC1-C5F08C039569}" type="CELLRANGE">
+                    <a:fld id="{98CDD4BF-2DBA-40A0-9A9A-421962D02AEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -23090,7 +23089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DAFC5A0-BF71-488D-985E-65F6A7FAAB85}" type="CELLRANGE">
+                    <a:fld id="{DE0B02E7-9B52-4EAB-8F94-E978875ADDFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -23124,7 +23123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E75B683C-F7EF-4369-88CA-783CF58C1805}" type="CELLRANGE">
+                    <a:fld id="{DABA5CE1-9456-44BC-841E-45293F0A53F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -28995,7 +28994,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{12FFEA56-D690-4F65-A8CE-5A70D0B0245D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -29094,7 +29093,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656674" cy="6282070"/>
+    <xdr:ext cx="8656320" cy="6278880"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -30359,7 +30358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>